<commit_message>
querys, bdd, cambios en tabla y peticiones ajax para tipo_vuelo
</commit_message>
<xml_diff>
--- a/EquiposYVuelos.xlsx
+++ b/EquiposYVuelos.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="186">
   <si>
     <t>Modelo</t>
   </si>
@@ -325,9 +325,6 @@
     <t>BUE</t>
   </si>
   <si>
-    <t>35días</t>
-  </si>
-  <si>
     <t>Entre Destinos</t>
   </si>
   <si>
@@ -494,13 +491,106 @@
   </si>
   <si>
     <t>Escalas</t>
+  </si>
+  <si>
+    <t>id_vuelo</t>
+  </si>
+  <si>
+    <t>duracion</t>
+  </si>
+  <si>
+    <t>fecha</t>
+  </si>
+  <si>
+    <t>cod_equipo</t>
+  </si>
+  <si>
+    <t>cod_tipo_vuelo</t>
+  </si>
+  <si>
+    <t>cod_trayecto</t>
+  </si>
+  <si>
+    <t>cod_estado</t>
+  </si>
+  <si>
+    <t>Guanaco (ids:35,36,37,38)</t>
+  </si>
+  <si>
+    <t>VUELO</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>id_equipo</t>
+  </si>
+  <si>
+    <t>RESERVA</t>
+  </si>
+  <si>
+    <t>id_reserva</t>
+  </si>
+  <si>
+    <t>cod_vuelo</t>
+  </si>
+  <si>
+    <t>cod_usuario</t>
+  </si>
+  <si>
+    <t>desde</t>
+  </si>
+  <si>
+    <t>hasta</t>
+  </si>
+  <si>
+    <t>ReTra</t>
+  </si>
+  <si>
+    <t>cod_reserva</t>
+  </si>
+  <si>
+    <t>id_retra</t>
+  </si>
+  <si>
+    <t>puerto</t>
+  </si>
+  <si>
+    <t>IO</t>
+  </si>
+  <si>
+    <t>Ganimedez</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>autonumerico</t>
+  </si>
+  <si>
+    <t>Pepe</t>
+  </si>
+  <si>
+    <t>lala</t>
+  </si>
+  <si>
+    <t>SubOrbital</t>
+  </si>
+  <si>
+    <t>Tipo_vuelo</t>
+  </si>
+  <si>
+    <t>12/15 - 25/29</t>
+  </si>
+  <si>
+    <t>35/39</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -508,8 +598,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -546,6 +651,54 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -574,7 +727,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -606,6 +759,28 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -894,7 +1069,7 @@
   <dimension ref="A2:Q47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,6 +1084,9 @@
       <c r="B2" t="s">
         <v>1</v>
       </c>
+      <c r="I2" t="s">
+        <v>183</v>
+      </c>
       <c r="J2" t="s">
         <v>5</v>
       </c>
@@ -936,7 +1114,7 @@
         <v>61</v>
       </c>
       <c r="J3" t="s">
-        <v>2</v>
+        <v>182</v>
       </c>
       <c r="K3" t="s">
         <v>3</v>
@@ -962,7 +1140,7 @@
         <v>65</v>
       </c>
       <c r="J4" t="s">
-        <v>2</v>
+        <v>182</v>
       </c>
       <c r="K4" t="s">
         <v>4</v>
@@ -1266,10 +1444,10 @@
         <v>24</v>
       </c>
       <c r="P19" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q19" s="8" t="s">
         <v>148</v>
-      </c>
-      <c r="Q19" s="8" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -1279,11 +1457,17 @@
       <c r="B20" t="s">
         <v>59</v>
       </c>
+      <c r="G20" t="s">
+        <v>184</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
       <c r="I20" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K20" s="8" t="s">
         <v>3</v>
@@ -1310,11 +1494,17 @@
       <c r="B21" t="s">
         <v>60</v>
       </c>
+      <c r="G21" t="s">
+        <v>184</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
       <c r="I21" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K21" s="8" t="s">
         <v>4</v>
@@ -1341,6 +1531,9 @@
       <c r="B22" t="s">
         <v>47</v>
       </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
       <c r="I22" s="8" t="s">
         <v>2</v>
       </c>
@@ -1372,6 +1565,9 @@
       <c r="B23" t="s">
         <v>48</v>
       </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
       <c r="I23" s="8" t="s">
         <v>2</v>
       </c>
@@ -1403,6 +1599,9 @@
       <c r="B24" t="s">
         <v>49</v>
       </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
       <c r="I24" s="8" t="s">
         <v>2</v>
       </c>
@@ -1434,6 +1633,9 @@
       <c r="B25" t="s">
         <v>50</v>
       </c>
+      <c r="H25">
+        <v>2</v>
+      </c>
       <c r="I25" s="8" t="s">
         <v>2</v>
       </c>
@@ -1465,6 +1667,9 @@
       <c r="B26" t="s">
         <v>37</v>
       </c>
+      <c r="H26">
+        <v>2</v>
+      </c>
       <c r="I26" s="8" t="s">
         <v>2</v>
       </c>
@@ -1496,6 +1701,9 @@
       <c r="B27" t="s">
         <v>38</v>
       </c>
+      <c r="H27">
+        <v>2</v>
+      </c>
       <c r="I27" s="8" t="s">
         <v>2</v>
       </c>
@@ -1527,6 +1735,9 @@
       <c r="B28" t="s">
         <v>39</v>
       </c>
+      <c r="H28">
+        <v>2</v>
+      </c>
       <c r="I28" s="8" t="s">
         <v>2</v>
       </c>
@@ -1558,6 +1769,9 @@
       <c r="B29" t="s">
         <v>42</v>
       </c>
+      <c r="H29">
+        <v>2</v>
+      </c>
       <c r="I29" s="8" t="s">
         <v>2</v>
       </c>
@@ -1606,7 +1820,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -1614,7 +1828,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>13</v>
       </c>
@@ -1622,7 +1836,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -1630,7 +1844,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>15</v>
       </c>
@@ -1649,8 +1863,11 @@
         <v>23</v>
       </c>
       <c r="L36" s="14"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M36" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>15</v>
       </c>
@@ -1669,8 +1886,11 @@
         <v>23</v>
       </c>
       <c r="L37" s="14"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M37" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>15</v>
       </c>
@@ -1689,8 +1909,11 @@
         <v>23</v>
       </c>
       <c r="L38" s="14"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M38" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>15</v>
       </c>
@@ -1709,8 +1932,11 @@
         <v>23</v>
       </c>
       <c r="L39" s="14"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M39" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -1718,7 +1944,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -1726,7 +1952,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -1734,7 +1960,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -1742,7 +1968,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -1750,7 +1976,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -1758,7 +1984,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>8</v>
       </c>
@@ -1766,7 +1992,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -1784,393 +2010,933 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I30"/>
+  <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="H4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="75.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="H1" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="M1" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="S1" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="U1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="H2" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="K2" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="V2" s="8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="H3" s="17">
+        <v>1</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="24">
+        <v>43789</v>
+      </c>
+      <c r="K3" s="17">
+        <v>2</v>
+      </c>
+      <c r="M3" s="17">
+        <v>1</v>
+      </c>
+      <c r="N3" s="17">
+        <v>1</v>
+      </c>
+      <c r="O3" s="17">
+        <v>39347706</v>
+      </c>
+      <c r="P3" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q3" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="S3" s="17">
+        <v>1</v>
+      </c>
+      <c r="T3" s="17">
+        <v>1</v>
+      </c>
+      <c r="U3" s="17">
+        <v>1</v>
+      </c>
+      <c r="V3" s="17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="8">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="8" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="S4" s="17">
+        <v>1</v>
+      </c>
+      <c r="T4" s="17">
+        <v>1</v>
+      </c>
+      <c r="U4" s="17">
+        <v>2</v>
+      </c>
+      <c r="V4" s="17" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="8">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="8" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="S5" s="17">
+        <v>1</v>
+      </c>
+      <c r="T5" s="17">
+        <v>1</v>
+      </c>
+      <c r="U5" s="17">
+        <v>3</v>
+      </c>
+      <c r="V5" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="8">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="8" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="H6" s="26">
+        <v>1</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="27">
+        <v>43789</v>
+      </c>
+      <c r="K6" s="26">
+        <v>2</v>
+      </c>
+      <c r="M6" s="26">
+        <v>2</v>
+      </c>
+      <c r="N6" s="26">
+        <v>1</v>
+      </c>
+      <c r="O6" s="26">
+        <v>1111111</v>
+      </c>
+      <c r="P6" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q6" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="S6" s="25">
+        <v>2</v>
+      </c>
+      <c r="T6" s="25">
+        <v>1</v>
+      </c>
+      <c r="U6" s="25">
+        <v>4</v>
+      </c>
+      <c r="V6" s="25" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="8">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="8" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="S7" s="25">
+        <v>2</v>
+      </c>
+      <c r="T7" s="25">
+        <v>1</v>
+      </c>
+      <c r="U7" s="25">
+        <v>5</v>
+      </c>
+      <c r="V7" s="25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="8">
         <v>5</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="8">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="8" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="H9" s="28">
+        <v>1</v>
+      </c>
+      <c r="I9" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="29">
+        <v>43789</v>
+      </c>
+      <c r="K9" s="28">
+        <v>2</v>
+      </c>
+      <c r="M9" s="28">
+        <v>3</v>
+      </c>
+      <c r="N9" s="28">
+        <v>1</v>
+      </c>
+      <c r="O9" s="28">
+        <v>2222222</v>
+      </c>
+      <c r="P9" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q9" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="S9" s="28">
+        <v>3</v>
+      </c>
+      <c r="T9" s="28">
+        <v>1</v>
+      </c>
+      <c r="U9" s="28">
+        <v>6</v>
+      </c>
+      <c r="V9" s="28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="8">
         <v>10</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="8" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="S10" s="28">
+        <v>3</v>
+      </c>
+      <c r="T10" s="28">
+        <v>1</v>
+      </c>
+      <c r="U10" s="28">
+        <v>7</v>
+      </c>
+      <c r="V10" s="28" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="H11" s="22">
+        <v>21</v>
+      </c>
+      <c r="I11" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="23">
+        <v>43810</v>
+      </c>
+      <c r="K11" s="22">
+        <v>2</v>
+      </c>
+      <c r="M11" s="22">
+        <v>4</v>
+      </c>
+      <c r="N11" s="22">
+        <v>21</v>
+      </c>
+      <c r="O11" s="22">
+        <v>90909090</v>
+      </c>
+      <c r="P11" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q11" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="S11" s="28">
+        <v>3</v>
+      </c>
+      <c r="T11" s="28">
+        <v>1</v>
+      </c>
+      <c r="U11" s="28">
+        <v>8</v>
+      </c>
+      <c r="V11" s="28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S12" s="28">
+        <v>3</v>
+      </c>
+      <c r="T12" s="28">
+        <v>1</v>
+      </c>
+      <c r="U12" s="28">
+        <v>9</v>
+      </c>
+      <c r="V12" s="28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="H13" s="31">
+        <v>3</v>
+      </c>
+      <c r="I13" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="J13" s="31">
+        <v>213123</v>
+      </c>
+      <c r="K13" s="31">
+        <v>2</v>
+      </c>
+      <c r="M13" s="31">
+        <v>5</v>
+      </c>
+      <c r="N13" s="31">
+        <v>3</v>
+      </c>
+      <c r="O13" s="31">
+        <v>123123123</v>
+      </c>
+      <c r="P13" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q13" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="S13" s="28">
+        <v>3</v>
+      </c>
+      <c r="T13" s="28">
+        <v>1</v>
+      </c>
+      <c r="U13" s="28">
+        <v>10</v>
+      </c>
+      <c r="V13" s="28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="E14" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="S14" s="28">
+        <v>3</v>
+      </c>
+      <c r="T14" s="28">
+        <v>1</v>
+      </c>
+      <c r="U14" s="28">
+        <v>11</v>
+      </c>
+      <c r="V14" s="28" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="S15" s="28"/>
+      <c r="T15" s="28"/>
+      <c r="U15" s="28"/>
+      <c r="V15" s="28"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="I16" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="J16" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="K16" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="L16" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="M16" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="N16" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="P16" s="33"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>155</v>
+      </c>
+      <c r="B17" t="s">
+        <v>156</v>
+      </c>
+      <c r="C17" t="s">
+        <v>157</v>
+      </c>
+      <c r="D17" t="s">
+        <v>158</v>
+      </c>
+      <c r="E17" t="s">
+        <v>159</v>
+      </c>
+      <c r="F17" t="s">
+        <v>160</v>
+      </c>
+      <c r="G17" t="s">
+        <v>161</v>
+      </c>
+      <c r="I17" s="8">
+        <v>1</v>
+      </c>
+      <c r="J17" s="8">
+        <v>1</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="L17" s="8">
+        <v>1</v>
+      </c>
+      <c r="M17" s="8">
+        <v>2</v>
+      </c>
+      <c r="N17" s="8">
+        <v>1</v>
+      </c>
+      <c r="P17" s="33"/>
+      <c r="S17" s="22">
+        <v>4</v>
+      </c>
+      <c r="T17" s="22">
+        <v>21</v>
+      </c>
+      <c r="U17" s="22">
+        <v>13</v>
+      </c>
+      <c r="V17" s="22" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <v>504</v>
+      </c>
+      <c r="C18" s="16">
+        <v>43807</v>
+      </c>
+      <c r="D18">
+        <v>35</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="I18" s="8">
+        <v>1</v>
+      </c>
+      <c r="J18" s="8">
+        <v>2</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="L18" s="8">
+        <v>1</v>
+      </c>
+      <c r="M18" s="8">
+        <v>2</v>
+      </c>
+      <c r="N18" s="8">
+        <v>1</v>
+      </c>
+      <c r="P18" s="33"/>
+      <c r="S18" s="22">
+        <v>4</v>
+      </c>
+      <c r="T18" s="22">
+        <v>21</v>
+      </c>
+      <c r="U18" s="22">
+        <v>14</v>
+      </c>
+      <c r="V18" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>504</v>
+      </c>
+      <c r="C19" s="16">
+        <v>43814</v>
+      </c>
+      <c r="D19">
+        <v>36</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="I19" s="8">
+        <v>1</v>
+      </c>
+      <c r="J19" s="8">
+        <v>3</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="L19" s="8">
+        <v>1</v>
+      </c>
+      <c r="M19" s="8">
+        <v>2</v>
+      </c>
+      <c r="N19" s="8">
+        <v>1</v>
+      </c>
+      <c r="O19" s="8"/>
+      <c r="P19" s="33"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="33"/>
+      <c r="S20" s="31">
+        <v>5</v>
+      </c>
+      <c r="T20" s="31">
+        <v>3</v>
+      </c>
+      <c r="U20" s="31">
+        <v>15</v>
+      </c>
+      <c r="V20" s="31" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="33"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="33"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B23" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="33"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="33"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="33"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B35" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I35" s="8"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="B24" t="s">
-        <v>113</v>
-      </c>
-      <c r="C24" t="s">
-        <v>114</v>
-      </c>
-      <c r="D24" t="s">
-        <v>115</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="C36" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="F24" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>112</v>
-      </c>
-      <c r="B25" t="s">
-        <v>117</v>
-      </c>
-      <c r="C25" t="s">
-        <v>114</v>
-      </c>
-      <c r="D25" t="s">
-        <v>118</v>
-      </c>
-      <c r="E25" t="s">
-        <v>119</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="C37" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="I37" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>106</v>
-      </c>
-      <c r="B26" t="s">
-        <v>102</v>
-      </c>
-      <c r="C26" t="s">
-        <v>104</v>
-      </c>
-      <c r="D26" t="s">
-        <v>107</v>
-      </c>
-      <c r="E26" t="s">
-        <v>108</v>
-      </c>
-      <c r="F26" t="s">
-        <v>109</v>
-      </c>
-      <c r="G26" t="s">
-        <v>110</v>
-      </c>
-      <c r="H26" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>112</v>
-      </c>
-      <c r="B27" t="s">
-        <v>113</v>
-      </c>
-      <c r="C27" t="s">
-        <v>125</v>
-      </c>
-      <c r="D27" t="s">
-        <v>120</v>
-      </c>
-      <c r="E27" t="s">
-        <v>121</v>
-      </c>
-      <c r="F27" t="s">
-        <v>122</v>
-      </c>
-      <c r="G27" t="s">
-        <v>123</v>
-      </c>
-      <c r="H27" t="s">
-        <v>124</v>
-      </c>
-      <c r="I27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>112</v>
-      </c>
-      <c r="B28" t="s">
-        <v>117</v>
-      </c>
-      <c r="C28" t="s">
-        <v>126</v>
-      </c>
-      <c r="D28" t="s">
-        <v>127</v>
-      </c>
-      <c r="E28" t="s">
-        <v>128</v>
-      </c>
-      <c r="F28" t="s">
-        <v>129</v>
-      </c>
-      <c r="G28" t="s">
-        <v>121</v>
-      </c>
-      <c r="H28" t="s">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="I28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>131</v>
-      </c>
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A42:E42"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2190,19 +2956,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>135</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2210,7 +2976,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="8"/>
@@ -2221,7 +2987,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="8"/>
@@ -2232,7 +2998,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="7"/>
@@ -2243,7 +3009,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="12"/>
@@ -2254,7 +3020,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="8"/>
@@ -2265,7 +3031,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="12"/>
@@ -2276,7 +3042,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -2287,7 +3053,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -2298,7 +3064,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="8"/>
@@ -2309,7 +3075,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>

</xml_diff>

<commit_message>
CAMBIO EN BDD, INSERTS VUELOS Y TRAYECTOS, VISTA DE VUELOS Y AJAX CAMBIADO
</commit_message>
<xml_diff>
--- a/EquiposYVuelos.xlsx
+++ b/EquiposYVuelos.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="185">
   <si>
     <t>Modelo</t>
   </si>
@@ -569,9 +569,6 @@
   </si>
   <si>
     <t>Pepe</t>
-  </si>
-  <si>
-    <t>lala</t>
   </si>
   <si>
     <t>SubOrbital</t>
@@ -700,7 +697,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -723,11 +720,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -759,9 +767,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -781,6 +786,10 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1069,7 +1078,7 @@
   <dimension ref="A2:Q47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,7 +1094,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J2" t="s">
         <v>5</v>
@@ -1114,7 +1123,7 @@
         <v>61</v>
       </c>
       <c r="J3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K3" t="s">
         <v>3</v>
@@ -1140,7 +1149,7 @@
         <v>65</v>
       </c>
       <c r="J4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K4" t="s">
         <v>4</v>
@@ -1458,7 +1467,7 @@
         <v>59</v>
       </c>
       <c r="G20" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -1495,7 +1504,7 @@
         <v>60</v>
       </c>
       <c r="G21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -1864,7 +1873,7 @@
       </c>
       <c r="L36" s="14"/>
       <c r="M36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -1887,7 +1896,7 @@
       </c>
       <c r="L37" s="14"/>
       <c r="M37" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -1910,7 +1919,7 @@
       </c>
       <c r="L38" s="14"/>
       <c r="M38" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -1933,7 +1942,7 @@
       </c>
       <c r="L39" s="14"/>
       <c r="M39" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -2010,10 +2019,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V42"/>
+  <dimension ref="A1:V35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2030,13 +2039,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="M1" s="19" t="s">
+      <c r="M1" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="S1" s="21" t="s">
+      <c r="S1" s="20" t="s">
         <v>172</v>
       </c>
       <c r="U1" t="s">
@@ -2044,7 +2053,7 @@
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="8"/>
@@ -2060,7 +2069,7 @@
       <c r="J2" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="K2" s="30" t="s">
+      <c r="K2" s="29" t="s">
         <v>159</v>
       </c>
       <c r="M2" s="8" t="s">
@@ -2079,13 +2088,13 @@
         <v>171</v>
       </c>
       <c r="S2" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="T2" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="U2" s="8" t="s">
-        <v>173</v>
+      <c r="U2" s="35" t="s">
+        <v>174</v>
       </c>
       <c r="V2" s="8" t="s">
         <v>175</v>
@@ -2107,43 +2116,43 @@
       <c r="E3" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="17">
+      <c r="H3" s="16">
         <v>1</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="24">
+      <c r="J3" s="23">
         <v>43789</v>
       </c>
-      <c r="K3" s="17">
+      <c r="K3" s="16">
         <v>2</v>
       </c>
-      <c r="M3" s="17">
+      <c r="M3" s="16">
         <v>1</v>
       </c>
-      <c r="N3" s="17">
+      <c r="N3" s="16">
         <v>1</v>
       </c>
-      <c r="O3" s="17">
+      <c r="O3" s="16">
         <v>39347706</v>
       </c>
-      <c r="P3" s="17" t="s">
+      <c r="P3" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="Q3" s="17" t="s">
+      <c r="Q3" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="S3" s="17">
+      <c r="S3" s="16">
         <v>1</v>
       </c>
-      <c r="T3" s="17">
+      <c r="T3" s="16">
         <v>1</v>
       </c>
-      <c r="U3" s="17">
+      <c r="U3" s="16">
         <v>1</v>
       </c>
-      <c r="V3" s="17" t="s">
+      <c r="V3" s="16" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2163,16 +2172,16 @@
       <c r="E4" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="S4" s="17">
+      <c r="S4" s="16">
         <v>1</v>
       </c>
-      <c r="T4" s="17">
+      <c r="T4" s="16">
         <v>1</v>
       </c>
-      <c r="U4" s="17">
+      <c r="U4" s="16">
         <v>2</v>
       </c>
-      <c r="V4" s="17" t="s">
+      <c r="V4" s="16" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2192,16 +2201,16 @@
       <c r="E5" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="S5" s="17">
+      <c r="S5" s="16">
         <v>1</v>
       </c>
-      <c r="T5" s="17">
+      <c r="T5" s="16">
         <v>1</v>
       </c>
-      <c r="U5" s="17">
+      <c r="U5" s="16">
         <v>3</v>
       </c>
-      <c r="V5" s="17" t="s">
+      <c r="V5" s="16" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2221,43 +2230,43 @@
       <c r="E6" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="H6" s="26">
+      <c r="H6" s="25">
         <v>1</v>
       </c>
-      <c r="I6" s="26" t="s">
+      <c r="I6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="27">
+      <c r="J6" s="26">
         <v>43789</v>
       </c>
-      <c r="K6" s="26">
+      <c r="K6" s="25">
         <v>2</v>
       </c>
-      <c r="M6" s="26">
+      <c r="M6" s="25">
         <v>2</v>
       </c>
-      <c r="N6" s="26">
+      <c r="N6" s="25">
         <v>1</v>
       </c>
-      <c r="O6" s="26">
+      <c r="O6" s="25">
         <v>1111111</v>
       </c>
-      <c r="P6" s="26" t="s">
+      <c r="P6" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="Q6" s="26" t="s">
+      <c r="Q6" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="S6" s="25">
+      <c r="S6" s="24">
         <v>2</v>
       </c>
-      <c r="T6" s="25">
+      <c r="T6" s="24">
         <v>1</v>
       </c>
-      <c r="U6" s="25">
+      <c r="U6" s="24">
         <v>4</v>
       </c>
-      <c r="V6" s="25" t="s">
+      <c r="V6" s="24" t="s">
         <v>178</v>
       </c>
     </row>
@@ -2277,16 +2286,16 @@
       <c r="E7" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="S7" s="25">
+      <c r="S7" s="24">
         <v>2</v>
       </c>
-      <c r="T7" s="25">
+      <c r="T7" s="24">
         <v>1</v>
       </c>
-      <c r="U7" s="25">
+      <c r="U7" s="24">
         <v>5</v>
       </c>
-      <c r="V7" s="25" t="s">
+      <c r="V7" s="24" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2323,43 +2332,43 @@
       <c r="E9" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="H9" s="28">
+      <c r="H9" s="27">
         <v>1</v>
       </c>
-      <c r="I9" s="28" t="s">
+      <c r="I9" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="29">
+      <c r="J9" s="28">
         <v>43789</v>
       </c>
-      <c r="K9" s="28">
+      <c r="K9" s="27">
         <v>2</v>
       </c>
-      <c r="M9" s="28">
+      <c r="M9" s="27">
         <v>3</v>
       </c>
-      <c r="N9" s="28">
+      <c r="N9" s="27">
         <v>1</v>
       </c>
-      <c r="O9" s="28">
+      <c r="O9" s="27">
         <v>2222222</v>
       </c>
-      <c r="P9" s="28" t="s">
+      <c r="P9" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="Q9" s="28" t="s">
+      <c r="Q9" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="S9" s="28">
+      <c r="S9" s="27">
         <v>3</v>
       </c>
-      <c r="T9" s="28">
+      <c r="T9" s="27">
         <v>1</v>
       </c>
-      <c r="U9" s="28">
+      <c r="U9" s="27">
         <v>6</v>
       </c>
-      <c r="V9" s="28" t="s">
+      <c r="V9" s="27" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2379,76 +2388,76 @@
       <c r="E10" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="S10" s="28">
+      <c r="S10" s="27">
         <v>3</v>
       </c>
-      <c r="T10" s="28">
+      <c r="T10" s="27">
         <v>1</v>
       </c>
-      <c r="U10" s="28">
+      <c r="U10" s="27">
         <v>7</v>
       </c>
-      <c r="V10" s="28" t="s">
+      <c r="V10" s="27" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="H11" s="22">
+      <c r="H11" s="21">
         <v>21</v>
       </c>
-      <c r="I11" s="22" t="s">
+      <c r="I11" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="J11" s="23">
+      <c r="J11" s="22">
         <v>43810</v>
       </c>
-      <c r="K11" s="22">
+      <c r="K11" s="21">
         <v>2</v>
       </c>
-      <c r="M11" s="22">
+      <c r="M11" s="21">
         <v>4</v>
       </c>
-      <c r="N11" s="22">
+      <c r="N11" s="21">
         <v>21</v>
       </c>
-      <c r="O11" s="22">
+      <c r="O11" s="21">
         <v>90909090</v>
       </c>
-      <c r="P11" s="22" t="s">
+      <c r="P11" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="Q11" s="22" t="s">
+      <c r="Q11" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="S11" s="28">
+      <c r="S11" s="27">
         <v>3</v>
       </c>
-      <c r="T11" s="28">
+      <c r="T11" s="27">
         <v>1</v>
       </c>
-      <c r="U11" s="28">
+      <c r="U11" s="27">
         <v>8</v>
       </c>
-      <c r="V11" s="28" t="s">
+      <c r="V11" s="27" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="S12" s="28">
+      <c r="S12" s="27">
         <v>3</v>
       </c>
-      <c r="T12" s="28">
+      <c r="T12" s="27">
         <v>1</v>
       </c>
-      <c r="U12" s="28">
+      <c r="U12" s="27">
         <v>9</v>
       </c>
-      <c r="V12" s="28" t="s">
+      <c r="V12" s="27" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="19" t="s">
         <v>97</v>
       </c>
       <c r="B13" s="8"/>
@@ -2456,43 +2465,43 @@
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
-      <c r="H13" s="31">
+      <c r="H13" s="30">
         <v>3</v>
       </c>
-      <c r="I13" s="31" t="s">
+      <c r="I13" s="30" t="s">
         <v>180</v>
       </c>
-      <c r="J13" s="31">
+      <c r="J13" s="30">
         <v>213123</v>
       </c>
-      <c r="K13" s="31">
+      <c r="K13" s="30">
         <v>2</v>
       </c>
-      <c r="M13" s="31">
+      <c r="M13" s="30">
         <v>5</v>
       </c>
-      <c r="N13" s="31">
+      <c r="N13" s="30">
         <v>3</v>
       </c>
-      <c r="O13" s="31">
+      <c r="O13" s="30">
         <v>123123123</v>
       </c>
-      <c r="P13" s="31" t="s">
+      <c r="P13" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="Q13" s="31" t="s">
+      <c r="Q13" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="S13" s="28">
+      <c r="S13" s="27">
         <v>3</v>
       </c>
-      <c r="T13" s="28">
+      <c r="T13" s="27">
         <v>1</v>
       </c>
-      <c r="U13" s="28">
+      <c r="U13" s="27">
         <v>10</v>
       </c>
-      <c r="V13" s="28" t="s">
+      <c r="V13" s="27" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2515,16 +2524,16 @@
       <c r="F14" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="S14" s="28">
+      <c r="S14" s="27">
         <v>3</v>
       </c>
-      <c r="T14" s="28">
+      <c r="T14" s="27">
         <v>1</v>
       </c>
-      <c r="U14" s="28">
+      <c r="U14" s="27">
         <v>11</v>
       </c>
-      <c r="V14" s="28" t="s">
+      <c r="V14" s="27" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2545,31 +2554,19 @@
       <c r="F15" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="S15" s="28"/>
-      <c r="T15" s="28"/>
-      <c r="U15" s="28"/>
-      <c r="V15" s="28"/>
+      <c r="S15" s="27"/>
+      <c r="T15" s="27"/>
+      <c r="U15" s="27"/>
+      <c r="V15" s="27"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="I16" s="34" t="s">
-        <v>155</v>
-      </c>
-      <c r="J16" s="34" t="s">
-        <v>160</v>
-      </c>
-      <c r="K16" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="L16" s="32" t="s">
-        <v>158</v>
-      </c>
-      <c r="M16" s="32" t="s">
-        <v>159</v>
-      </c>
-      <c r="N16" s="32" t="s">
-        <v>161</v>
-      </c>
-      <c r="P16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="31"/>
+      <c r="P16" s="32"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -2593,35 +2590,23 @@
       <c r="G17" t="s">
         <v>161</v>
       </c>
-      <c r="I17" s="8">
-        <v>1</v>
-      </c>
-      <c r="J17" s="8">
-        <v>1</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="L17" s="8">
-        <v>1</v>
-      </c>
-      <c r="M17" s="8">
-        <v>2</v>
-      </c>
-      <c r="N17" s="8">
-        <v>1</v>
-      </c>
-      <c r="P17" s="33"/>
-      <c r="S17" s="22">
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="P17" s="32"/>
+      <c r="S17" s="21">
         <v>4</v>
       </c>
-      <c r="T17" s="22">
+      <c r="T17" s="21">
         <v>21</v>
       </c>
-      <c r="U17" s="22">
+      <c r="U17" s="21">
         <v>13</v>
       </c>
-      <c r="V17" s="22" t="s">
+      <c r="V17" s="21" t="s">
         <v>176</v>
       </c>
     </row>
@@ -2632,7 +2617,7 @@
       <c r="B18">
         <v>504</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="15">
         <v>43807</v>
       </c>
       <c r="D18">
@@ -2641,35 +2626,23 @@
       <c r="E18">
         <v>2</v>
       </c>
-      <c r="I18" s="8">
-        <v>1</v>
-      </c>
-      <c r="J18" s="8">
-        <v>2</v>
-      </c>
-      <c r="K18" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="L18" s="8">
-        <v>1</v>
-      </c>
-      <c r="M18" s="8">
-        <v>2</v>
-      </c>
-      <c r="N18" s="8">
-        <v>1</v>
-      </c>
-      <c r="P18" s="33"/>
-      <c r="S18" s="22">
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="P18" s="32"/>
+      <c r="S18" s="21">
         <v>4</v>
       </c>
-      <c r="T18" s="22">
+      <c r="T18" s="21">
         <v>21</v>
       </c>
-      <c r="U18" s="22">
+      <c r="U18" s="21">
         <v>14</v>
       </c>
-      <c r="V18" s="22" t="s">
+      <c r="V18" s="21" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2680,7 +2653,7 @@
       <c r="B19">
         <v>504</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19" s="15">
         <v>43814</v>
       </c>
       <c r="D19">
@@ -2689,26 +2662,14 @@
       <c r="E19">
         <v>2</v>
       </c>
-      <c r="I19" s="8">
-        <v>1</v>
-      </c>
-      <c r="J19" s="8">
-        <v>3</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="L19" s="8">
-        <v>1</v>
-      </c>
-      <c r="M19" s="8">
-        <v>2</v>
-      </c>
-      <c r="N19" s="8">
-        <v>1</v>
-      </c>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
       <c r="O19" s="8"/>
-      <c r="P19" s="33"/>
+      <c r="P19" s="32"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="I20" s="8"/>
@@ -2718,17 +2679,17 @@
       <c r="M20" s="8"/>
       <c r="N20" s="8"/>
       <c r="O20" s="8"/>
-      <c r="P20" s="33"/>
-      <c r="S20" s="31">
+      <c r="P20" s="32"/>
+      <c r="S20" s="30">
         <v>5</v>
       </c>
-      <c r="T20" s="31">
+      <c r="T20" s="30">
         <v>3</v>
       </c>
-      <c r="U20" s="31">
+      <c r="U20" s="30">
         <v>15</v>
       </c>
-      <c r="V20" s="31" t="s">
+      <c r="V20" s="30" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2740,10 +2701,10 @@
       <c r="M21" s="8"/>
       <c r="N21" s="8"/>
       <c r="O21" s="8"/>
-      <c r="P21" s="33"/>
+      <c r="P21" s="32"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="17" t="s">
         <v>99</v>
       </c>
       <c r="I22" s="8"/>
@@ -2753,7 +2714,7 @@
       <c r="M22" s="8"/>
       <c r="N22" s="8"/>
       <c r="O22" s="8"/>
-      <c r="P22" s="33"/>
+      <c r="P22" s="32"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
@@ -2779,7 +2740,7 @@
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
       <c r="O23" s="8"/>
-      <c r="P23" s="33"/>
+      <c r="P23" s="32"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
@@ -2807,7 +2768,7 @@
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
       <c r="O24" s="8"/>
-      <c r="P24" s="33"/>
+      <c r="P24" s="32"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
@@ -2835,105 +2796,105 @@
       <c r="M25" s="8"/>
       <c r="N25" s="8"/>
       <c r="O25" s="8"/>
-      <c r="P25" s="33"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+      <c r="P25" s="32"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B28" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C28" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D28" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E28" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="F28" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="G28" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="H28" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="I35" s="8"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+      <c r="I28" s="8"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B29" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C29" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D29" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E29" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="F29" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G36" s="8" t="s">
+      <c r="G29" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="H36" s="8" t="s">
+      <c r="H29" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="I36" s="8" t="s">
+      <c r="I29" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B30" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C30" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D30" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E30" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="F30" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="G37" s="8" t="s">
+      <c r="G30" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="H37" s="8" t="s">
+      <c r="H30" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="I37" s="8" t="s">
+      <c r="I30" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="A35:E35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2945,7 +2906,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3012,7 +2973,7 @@
         <v>139</v>
       </c>
       <c r="C5" s="8"/>
-      <c r="D5" s="12"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">

</xml_diff>